<commit_message>
Sauvegarde des dernières modifications
</commit_message>
<xml_diff>
--- a/Base de données.xlsx
+++ b/Base de données.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vincienergies-my.sharepoint.com/personal/nada_zennaba_vinci-energies_net/Documents/Bureau/Streamlit code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vincienergies-my.sharepoint.com/personal/nada_zennaba_vinci-energies_net/Documents/Bureau/v5 - Copie (3)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="8_{31095B59-BD5B-4520-B519-0223138AA96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{843034D6-5BB0-4950-9DEB-9A188AE93C0A}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{31095B59-BD5B-4520-B519-0223138AA96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35F1DFCB-6499-43F8-8CD3-9FB8BF60B6AF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{81F2DBB1-46FB-42FE-8514-87645613A4B9}"/>
+    <workbookView xWindow="-8910" yWindow="-19305" windowWidth="28035" windowHeight="14850" xr2:uid="{81F2DBB1-46FB-42FE-8514-87645613A4B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Matériel" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,6 +580,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -594,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -625,15 +631,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1535,10 +1545,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FBE09822-D4F0-4DE9-8DFC-FE60D11FBA65}" name="Tableau3" displayName="Tableau3" ref="A1:E11" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:E11" xr:uid="{CAC5356E-0F07-4F2F-9536-26BC4818E4CA}"/>
@@ -1867,10 +1873,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356A5014-4925-4601-B5A9-BAAEF701CE55}">
   <sheetPr codeName="Feuil2" filterMode="1"/>
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:H70"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1930,11 +1936,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1958,15 +1964,15 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1990,15 +1996,15 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="15" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:13" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -2023,15 +2029,15 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -2056,13 +2062,13 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="M5" s="15"/>
+    </row>
+    <row r="6" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -2087,13 +2093,13 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="16"/>
-    </row>
-    <row r="7" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -2118,13 +2124,13 @@
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="16"/>
-    </row>
-    <row r="8" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -2148,15 +2154,15 @@
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -2180,15 +2186,15 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -2213,15 +2219,15 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -2246,15 +2252,15 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="16" t="s">
+      <c r="M11" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="15" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -2283,15 +2289,15 @@
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -2315,15 +2321,15 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -2347,18 +2353,16 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="16"/>
-    </row>
-    <row r="15" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
         <v>16</v>
       </c>
@@ -2369,24 +2373,20 @@
         <v>18</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="13">
-        <v>200</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H15" s="16"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="15" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="15" t="s">
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -2396,7 +2396,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>18</v>
@@ -2405,25 +2405,25 @@
         <v>19</v>
       </c>
       <c r="H16" s="13">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
-      <c r="M16" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M16" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>16</v>
@@ -2432,27 +2432,27 @@
         <v>18</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H17" s="13">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="15" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="M17" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -2471,84 +2471,87 @@
         <v>37</v>
       </c>
       <c r="H18" s="13">
-        <v>750</v>
+        <v>20</v>
       </c>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="M18" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="H19" s="13">
-        <v>40</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="15" t="s">
+      <c r="M19" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" s="13">
-        <v>6</v>
-      </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="16"/>
-    </row>
-    <row r="21" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="15" t="s">
+      <c r="C20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="4">
+        <v>225</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -2564,22 +2567,23 @@
         <v>18</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21" s="13">
-        <v>4</v>
-      </c>
-      <c r="I21" s="13"/>
+        <v>40</v>
+      </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
-      <c r="M21" s="16"/>
-    </row>
-    <row r="22" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M21" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -2604,15 +2608,15 @@
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="16" t="s">
+      <c r="M22" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -2637,15 +2641,15 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="16" t="s">
+      <c r="M23" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -2670,15 +2674,15 @@
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="16" t="s">
+      <c r="M24" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="13" t="s">
@@ -2703,15 +2707,15 @@
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="16" t="s">
+      <c r="M25" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
+    <row r="26" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -2736,13 +2740,13 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="16"/>
-    </row>
-    <row r="27" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
+      <c r="M26" s="15"/>
+    </row>
+    <row r="27" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -2767,15 +2771,15 @@
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="16" t="s">
+      <c r="M27" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
+    <row r="28" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -2800,15 +2804,15 @@
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
-      <c r="M28" s="16" t="s">
+      <c r="M28" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -2833,15 +2837,15 @@
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="16" t="s">
+      <c r="M29" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="13" t="s">
@@ -2866,15 +2870,15 @@
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
-      <c r="M30" s="16" t="s">
+      <c r="M30" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -2899,15 +2903,15 @@
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
-      <c r="M31" s="16" t="s">
+      <c r="M31" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -2932,15 +2936,15 @@
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
-      <c r="M32" s="16" t="s">
+      <c r="M32" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="13" t="s">
@@ -2965,15 +2969,15 @@
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
-      <c r="M33" s="16" t="s">
+      <c r="M33" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="15" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" s="14" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C34" s="13" t="s">
@@ -2998,15 +3002,15 @@
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
-      <c r="M34" s="16" t="s">
+      <c r="M34" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="13" t="s">
@@ -3031,15 +3035,15 @@
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
-      <c r="M35" s="16" t="s">
+      <c r="M35" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C36" s="13" t="s">
@@ -3064,15 +3068,15 @@
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
-      <c r="M36" s="16" t="s">
+      <c r="M36" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="13" t="s">
@@ -3097,15 +3101,15 @@
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
-      <c r="M37" s="16" t="s">
+      <c r="M37" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="13" t="s">
@@ -3130,15 +3134,15 @@
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
-      <c r="M38" s="16" t="s">
+      <c r="M38" s="15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C39" s="13" t="s">
@@ -3163,15 +3167,15 @@
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="16" t="s">
+      <c r="M39" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="15" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" s="14" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C40" s="13" t="s">
@@ -3196,15 +3200,15 @@
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
-      <c r="M40" s="16" t="s">
+      <c r="M40" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C41" s="13" t="s">
@@ -3229,15 +3233,15 @@
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
-      <c r="M41" s="16" t="s">
+      <c r="M41" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C42" s="13" t="s">
@@ -3262,15 +3266,15 @@
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
-      <c r="M42" s="16" t="s">
+      <c r="M42" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
+    <row r="43" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C43" s="13" t="s">
@@ -3295,15 +3299,15 @@
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
-      <c r="M43" s="16" t="s">
+      <c r="M43" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="16" t="s">
+    <row r="44" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C44" s="13" t="s">
@@ -3328,15 +3332,15 @@
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
-      <c r="M44" s="16" t="s">
+      <c r="M44" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="16" t="s">
+    <row r="45" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C45" s="13" t="s">
@@ -3361,15 +3365,15 @@
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
-      <c r="M45" s="16" t="s">
+      <c r="M45" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="15" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" s="14" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C46" s="13" t="s">
@@ -3394,15 +3398,15 @@
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
-      <c r="M46" s="16" t="s">
+      <c r="M46" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C47" s="13" t="s">
@@ -3427,13 +3431,13 @@
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
-      <c r="M47" s="16"/>
-    </row>
-    <row r="48" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M47" s="15"/>
+    </row>
+    <row r="48" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C48" s="13" t="s">
@@ -3458,13 +3462,13 @@
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
-      <c r="M48" s="16"/>
-    </row>
-    <row r="49" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M48" s="15"/>
+    </row>
+    <row r="49" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C49" s="13" t="s">
@@ -3489,15 +3493,15 @@
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
-      <c r="M49" s="16" t="s">
+      <c r="M49" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C50" s="13" t="s">
@@ -3522,13 +3526,13 @@
       <c r="J50" s="13"/>
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
-      <c r="M50" s="16"/>
-    </row>
-    <row r="51" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M50" s="15"/>
+    </row>
+    <row r="51" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C51" s="13" t="s">
@@ -3553,15 +3557,15 @@
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
-      <c r="M51" s="16" t="s">
+      <c r="M51" s="15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C52" s="13" t="s">
@@ -3586,13 +3590,13 @@
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
-      <c r="M52" s="16"/>
-    </row>
-    <row r="53" spans="1:13" s="15" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M52" s="15"/>
+    </row>
+    <row r="53" spans="1:13" s="14" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C53" s="13" t="s">
@@ -3621,15 +3625,15 @@
       </c>
       <c r="K53" s="13"/>
       <c r="L53" s="13"/>
-      <c r="M53" s="16" t="s">
+      <c r="M53" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C54" s="13" t="s">
@@ -3654,15 +3658,15 @@
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
-      <c r="M54" s="16" t="s">
+      <c r="M54" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C55" s="13" t="s">
@@ -3687,13 +3691,13 @@
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
-      <c r="M55" s="16"/>
-    </row>
-    <row r="56" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M55" s="15"/>
+    </row>
+    <row r="56" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C56" s="13" t="s">
@@ -3718,13 +3722,13 @@
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
-      <c r="M56" s="16"/>
-    </row>
-    <row r="57" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M56" s="15"/>
+    </row>
+    <row r="57" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C57" s="13" t="s">
@@ -3749,13 +3753,13 @@
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
-      <c r="M57" s="16"/>
-    </row>
-    <row r="58" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M57" s="15"/>
+    </row>
+    <row r="58" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="13" t="s">
@@ -3780,13 +3784,13 @@
       <c r="J58" s="13"/>
       <c r="K58" s="13"/>
       <c r="L58" s="13"/>
-      <c r="M58" s="16"/>
-    </row>
-    <row r="59" spans="1:13" s="15" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M58" s="15"/>
+    </row>
+    <row r="59" spans="1:13" s="14" customFormat="1" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C59" s="13" t="s">
@@ -3811,15 +3815,15 @@
       <c r="J59" s="13"/>
       <c r="K59" s="13"/>
       <c r="L59" s="13"/>
-      <c r="M59" s="16" t="s">
+      <c r="M59" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C60" s="13" t="s">
@@ -3844,13 +3848,13 @@
       <c r="J60" s="13"/>
       <c r="K60" s="13"/>
       <c r="L60" s="13"/>
-      <c r="M60" s="16"/>
-    </row>
-    <row r="61" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C61" s="13" t="s">
@@ -3875,13 +3879,13 @@
       <c r="J61" s="13"/>
       <c r="K61" s="13"/>
       <c r="L61" s="13"/>
-      <c r="M61" s="16"/>
-    </row>
-    <row r="62" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M61" s="15"/>
+    </row>
+    <row r="62" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C62" s="13" t="s">
@@ -3906,13 +3910,13 @@
       <c r="J62" s="13"/>
       <c r="K62" s="13"/>
       <c r="L62" s="13"/>
-      <c r="M62" s="16"/>
-    </row>
-    <row r="63" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M62" s="15"/>
+    </row>
+    <row r="63" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C63" s="13" t="s">
@@ -3937,13 +3941,13 @@
       <c r="J63" s="13"/>
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
-      <c r="M63" s="16"/>
-    </row>
-    <row r="64" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M63" s="15"/>
+    </row>
+    <row r="64" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C64" s="13" t="s">
@@ -3968,13 +3972,13 @@
       <c r="J64" s="13"/>
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
-      <c r="M64" s="16"/>
-    </row>
-    <row r="65" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M64" s="15"/>
+    </row>
+    <row r="65" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C65" s="13" t="s">
@@ -3999,13 +4003,13 @@
       <c r="J65" s="13"/>
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
-      <c r="M65" s="16"/>
-    </row>
-    <row r="66" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M65" s="15"/>
+    </row>
+    <row r="66" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C66" s="13" t="s">
@@ -4030,13 +4034,13 @@
       <c r="J66" s="13"/>
       <c r="K66" s="13"/>
       <c r="L66" s="13"/>
-      <c r="M66" s="16"/>
-    </row>
-    <row r="67" spans="1:13" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M66" s="15"/>
+    </row>
+    <row r="67" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C67" s="13" t="s">
@@ -4061,76 +4065,87 @@
       <c r="J67" s="13"/>
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
-      <c r="M67" s="16"/>
-    </row>
-    <row r="68" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M67" s="15"/>
+    </row>
+    <row r="68" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B68" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C68" s="13"/>
+      <c r="C68" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="D68" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F68" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H68" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="H68" s="13">
+        <v>6</v>
+      </c>
       <c r="I68" s="13"/>
       <c r="J68" s="13"/>
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
-      <c r="M68" s="16"/>
-    </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="M68" s="15"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A69" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H69" s="4">
-        <v>225</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C69" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H69" s="13">
+        <v>4</v>
+      </c>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="15"/>
+    </row>
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>151</v>
       </c>
     </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B91" s="17"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M70" xr:uid="{356A5014-4925-4601-B5A9-BAAEF701CE55}">
-    <filterColumn colId="7">
-      <filters blank="1"/>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="CVCD"/>
+      </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A68:M70">
-      <sortCondition descending="1" ref="A1:A70"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M69">
+      <sortCondition ref="A1:A70"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>